<commit_message>
Documents committed. (HP PC)
</commit_message>
<xml_diff>
--- a/myanmarentreprogrammer/002 Articles/I am going to Crate Blogging Platform in Java/01 RD/draft design/draft_design.xlsx
+++ b/myanmarentreprogrammer/002 Articles/I am going to Crate Blogging Platform in Java/01 RD/draft design/draft_design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Myanmar Simple Programmer (MSP)</t>
   </si>
@@ -220,12 +220,15 @@
   <si>
     <t>&lt;/div&gt;</t>
   </si>
+  <si>
+    <t>"I'm not talented, I'm obsessed."</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +281,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -400,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -418,6 +428,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,13 +830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K30"/>
+  <dimension ref="B3:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
@@ -832,7 +845,7 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -840,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="21">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -848,19 +861,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" ht="21">
       <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="21">
       <c r="B6" s="1"/>
       <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="21">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -883,7 +896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="21">
       <c r="B8" s="1"/>
       <c r="E8" s="2" t="s">
         <v>27</v>
@@ -892,7 +905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" ht="21">
       <c r="B9" s="1"/>
       <c r="E9" s="2" t="s">
         <v>2</v>
@@ -901,13 +914,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" ht="21">
       <c r="B10" s="1"/>
       <c r="E10" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" ht="21">
       <c r="B11" s="1"/>
       <c r="F11" s="3" t="s">
         <v>10</v>
@@ -915,7 +928,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" ht="21">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -924,8 +937,11 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="21">
       <c r="B13" s="1"/>
       <c r="C13" t="s">
         <v>34</v>
@@ -936,15 +952,18 @@
       </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:15" ht="21">
       <c r="B14" s="1"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="O14" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="21">
       <c r="B15" s="1"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
@@ -952,7 +971,7 @@
       </c>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" ht="21">
       <c r="B16" s="1"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7" t="s">
@@ -960,7 +979,7 @@
       </c>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="21">
       <c r="B17" s="1"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
@@ -968,7 +987,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="21">
       <c r="B18" s="1"/>
       <c r="F18" s="6">
         <v>2017</v>
@@ -976,7 +995,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="21">
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
@@ -986,40 +1005,40 @@
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="F20" s="6"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10">
       <c r="F23" s="6"/>
       <c r="G23" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10">
       <c r="F24" s="9"/>
       <c r="G24" s="10"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10">
       <c r="I27">
         <v>1</v>
       </c>
@@ -1027,17 +1046,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10">
       <c r="J28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10">
       <c r="J29" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10">
       <c r="J30" t="s">
         <v>23</v>
       </c>
@@ -1056,24 +1075,24 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" ht="21">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="21">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="21">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="21">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1087,42 +1106,42 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="21">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="21">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" ht="21">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="21">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" ht="21">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="21">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" ht="21">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" ht="21">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="21">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" ht="21">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="21">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="21">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1136,18 +1155,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D151:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+    <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="N170" sqref="N170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="151" spans="4:10" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="151" spans="4:10" ht="26.25">
       <c r="D151" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:10">
       <c r="I156">
         <v>1</v>
       </c>
@@ -1155,12 +1174,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="157" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:10">
       <c r="J157" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="158" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:10">
       <c r="I158">
         <v>2</v>
       </c>
@@ -1168,97 +1187,97 @@
         <v>39</v>
       </c>
     </row>
-    <row r="159" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:10">
       <c r="J159" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="164" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:11">
       <c r="D164" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="165" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:11">
       <c r="F165" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="166" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:11">
       <c r="G166" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="167" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:11">
       <c r="H167" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="168" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:11">
       <c r="I168" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:11">
       <c r="J169" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="170" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="4:11">
       <c r="K170" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="171" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:11">
       <c r="J171" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="172" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:11">
       <c r="I172" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="173" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:11">
       <c r="I173" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="174" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:11">
       <c r="J174" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:11">
       <c r="K175" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="176" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:11">
       <c r="K176" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="177" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:9">
       <c r="I177" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="178" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:9">
       <c r="H178" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="180" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:9">
       <c r="G180" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="181" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:9">
       <c r="F181" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="182" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:9">
       <c r="E182" t="s">
         <v>56</v>
       </c>
@@ -1278,13 +1297,13 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -1294,12 +1313,12 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7">
       <c r="G6" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7">
       <c r="C7" t="s">
         <v>31</v>
       </c>

</xml_diff>